<commit_message>
Update PCBA files & tutorials
</commit_message>
<xml_diff>
--- a/PCBs/IRD_PCB_4_1/BOM_SMT_TB_RFM95_868_IISS_PCB4_1_wH2.xlsx
+++ b/PCBs/IRD_PCB_4_1/BOM_SMT_TB_RFM95_868_IISS_PCB4_1_wH2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Documents/TEX/Pau-05/PROJET-PRIMA-INTELIRRIS/PCBs/IRD-JFP/V4.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19413944-5CCB-8D47-B77D-9A435FA0797F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F059D40-995A-3240-A2FB-D627E65CB473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -175,24 +175,6 @@
     <t>RF1</t>
   </si>
   <si>
-    <t>XY308-2.54-2P</t>
-  </si>
-  <si>
-    <t>C557685</t>
-  </si>
-  <si>
-    <t>XY308-2.54-3P</t>
-  </si>
-  <si>
-    <t>C557686</t>
-  </si>
-  <si>
-    <t>XY308-2.54-4P</t>
-  </si>
-  <si>
-    <t>C915913</t>
-  </si>
-  <si>
     <t>DL-RFM95-868M</t>
   </si>
   <si>
@@ -205,16 +187,10 @@
     <t>12P_F</t>
   </si>
   <si>
-    <t>CONN-TH_XY308-2.54-4P</t>
-  </si>
-  <si>
     <t>2P_F</t>
   </si>
   <si>
     <t>3P_F</t>
-  </si>
-  <si>
-    <t>CONN-TH_XY308-2.54-3P</t>
   </si>
   <si>
     <t>SMA-SMD_HJ-SMA716</t>
@@ -317,12 +293,6 @@
     <t>C492403</t>
   </si>
   <si>
-    <t>CN2</t>
-  </si>
-  <si>
-    <t>CN6,CN7,CN8</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -336,6 +306,27 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>C915916</t>
+  </si>
+  <si>
+    <t>CONN-TH_XY308-2.54-7P</t>
+  </si>
+  <si>
+    <t>CN8</t>
+  </si>
+  <si>
+    <t>XY308-2.54-6P</t>
+  </si>
+  <si>
+    <t>XY308-2.54-7P</t>
+  </si>
+  <si>
+    <t>CONN-TH_XY308-2.54-6P</t>
+  </si>
+  <si>
+    <t>C915915</t>
   </si>
 </sst>
 </file>
@@ -815,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -844,10 +835,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1">
@@ -879,7 +870,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>7</v>
@@ -894,7 +885,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="15">
-        <f t="shared" ref="H3:H24" si="0">F3/G3</f>
+        <f t="shared" ref="H3:H23" si="0">F3/G3</f>
         <v>9.0124999999999997E-2</v>
       </c>
     </row>
@@ -949,7 +940,7 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>13</v>
@@ -973,7 +964,7 @@
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>15</v>
@@ -1021,16 +1012,16 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F9" s="16">
         <v>2.4E-2</v>
@@ -1120,7 +1111,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>30</v>
@@ -1141,16 +1132,16 @@
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F14" s="13">
         <v>0.11700000000000001</v>
@@ -1165,16 +1156,16 @@
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F15" s="13">
         <v>0.45800000000000002</v>
@@ -1191,7 +1182,7 @@
         <v>6.85</v>
       </c>
       <c r="K15" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1">
@@ -1200,16 +1191,16 @@
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F17" s="13">
         <v>42.75</v>
@@ -1230,10 +1221,10 @@
         <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F18" s="13">
         <v>6.3179999999999996</v>
@@ -1248,16 +1239,16 @@
     </row>
     <row r="19" spans="1:11" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="F19" s="13">
         <v>5.2679999999999998</v>
@@ -1272,139 +1263,140 @@
     </row>
     <row r="20" spans="1:11" ht="20" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F20" s="13">
-        <v>2.6640000000000001</v>
+        <v>2.8180000000000001</v>
       </c>
       <c r="G20" s="1">
         <v>10</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="0"/>
-        <v>0.26640000000000003</v>
+        <v>0.28179999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>42</v>
+      <c r="A21" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="13">
-        <v>2.8180000000000001</v>
+        <v>69</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="16">
+        <v>1.8</v>
       </c>
       <c r="G21" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H21" s="15">
         <f t="shared" si="0"/>
-        <v>0.28179999999999999</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="20" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>76</v>
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="16">
-        <v>1.8</v>
+      <c r="F22" s="13">
+        <v>0.86699999999999999</v>
       </c>
       <c r="G22" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H22" s="15">
         <f t="shared" si="0"/>
-        <v>0.09</v>
+        <v>7.8818181818181815E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="13">
-        <v>0.86699999999999999</v>
+      <c r="F23" s="16">
+        <v>0.66</v>
       </c>
       <c r="G23" s="1">
         <v>11</v>
       </c>
       <c r="H23" s="15">
         <f t="shared" si="0"/>
-        <v>7.8818181818181815E-2</v>
+        <v>6.0000000000000005E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="16">
-        <v>0.66</v>
+      <c r="F24" s="1">
+        <v>0.20300000000000001</v>
       </c>
       <c r="G24" s="1">
         <v>11</v>
       </c>
       <c r="H24" s="15">
-        <f t="shared" si="0"/>
-        <v>6.0000000000000005E-2</v>
+        <f t="shared" ref="H24" si="1">F24/G24</f>
+        <v>1.8454545454545456E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
@@ -1414,64 +1406,39 @@
         <v>11</v>
       </c>
       <c r="H25" s="15">
-        <f t="shared" ref="H25" si="1">F25/G25</f>
+        <f t="shared" ref="H25" si="2">F25/G25</f>
         <v>1.8454545454545456E-2</v>
       </c>
+      <c r="J25">
+        <f>SUM(F17:F25)</f>
+        <v>60.886999999999993</v>
+      </c>
+      <c r="K25" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="20" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="G26" s="1">
-        <v>11</v>
-      </c>
-      <c r="H26" s="15">
-        <f t="shared" ref="H26" si="2">F26/G26</f>
-        <v>1.8454545454545456E-2</v>
-      </c>
-      <c r="J26">
-        <f>SUM(F17:F26)</f>
-        <v>63.550999999999995</v>
-      </c>
-      <c r="K26" t="s">
-        <v>79</v>
-      </c>
+      <c r="A26" s="11"/>
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="20" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="20" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" ht="20" customHeight="1">
-      <c r="F29" s="12">
-        <f>SUM(F2:F26)</f>
-        <v>70.40100000000001</v>
-      </c>
-      <c r="G29" s="14">
-        <f>F29/10</f>
-        <v>7.0401000000000007</v>
-      </c>
-      <c r="K29" t="s">
-        <v>80</v>
+      <c r="F28" s="12">
+        <f>SUM(F2:F25)</f>
+        <v>67.737000000000009</v>
+      </c>
+      <c r="G28" s="14">
+        <f>F28/10</f>
+        <v>6.7737000000000007</v>
+      </c>
+      <c r="K28" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>